<commit_message>
Changed layout, added 3d models
</commit_message>
<xml_diff>
--- a/Switches n stuff.xlsx
+++ b/Switches n stuff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikster\Desktop\LHR\Controls-DashboardPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E24666-DE6C-4136-AE80-7C5FB602E75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B0346-6691-401C-806E-3AB64DB90F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3591" yWindow="4397" windowWidth="20572" windowHeight="12026" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Indicator switch</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/c-k/A10305RNZQ/2055101</t>
+  </si>
+  <si>
+    <t>Amazon.com: Yohii 40 Pcs DC 50V 0.5A 3 Position Vertical Slide Switch 4 Pin SS13F11 Solder Lug Pin- (G7.23) : Industrial &amp; Scientific</t>
   </si>
 </sst>
 </file>
@@ -141,9 +144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,78 +374,80 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -464,6 +470,7 @@
     <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C5" r:id="rId5" xr:uid="{84ED3337-AE64-4A5C-81B7-8881D7D5F3CA}"/>
+    <hyperlink ref="H1" r:id="rId6" display="https://www.amazon.com/Yohii-Position-Vertical-Switch-SS13F11/dp/B07DNY27QB/ref=sr_1_11?crid=37FHDP7FPF998&amp;dib=eyJ2IjoiMSJ9.TmZHZGk3Hvvx_lyV6egheLU8wpUW1gQXKpK-pVoJM0YZhkksUHUBJKWiqwUQi9bXQUORBZ2FODAFGmqAx6kqR6BlfXK0BtXjfCogJMSNTGW_MvnyhMWbwwaFqZ6fDFfCzxAb2L5atYpxXBCXKbFj6BSlr-hKSALaJ9IvesXQGrzCAYdJ6u8L8nnwryZ1bUGBm8-7ZAXqObLHUMq_ZAx0SIk7rcdBataxrNZY30aDggI.Qg3lDAXLtPyvzHrJ3-Vu5ofHJ0HbOo4L6fDoAegk49o&amp;dib_tag=se&amp;keywords=large+3+position+slide+switch&amp;qid=1732387852&amp;sprefix=large3+position+slide+switch%2Caps%2C136&amp;sr=8-11" xr:uid="{A4D9C4F5-2B3F-415B-AF42-A7DA6814405E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some extra stuff and things
</commit_message>
<xml_diff>
--- a/Switches n stuff.xlsx
+++ b/Switches n stuff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikster\Desktop\LHR\Controls-DashboardPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B0346-6691-401C-806E-3AB64DB90F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20438D2-CDCB-41A0-88E4-379B29085445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Indicator switch</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Amazon.com: Yohii 40 Pcs DC 50V 0.5A 3 Position Vertical Slide Switch 4 Pin SS13F11 Solder Lug Pin- (G7.23) : Industrial &amp; Scientific</t>
+  </si>
+  <si>
+    <t>JN2UEENAGX E-Switch | Mouser</t>
   </si>
 </sst>
 </file>
@@ -371,15 +374,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -395,7 +398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -408,8 +411,11 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -423,7 +429,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -437,7 +443,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -471,6 +477,7 @@
     <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C5" r:id="rId5" xr:uid="{84ED3337-AE64-4A5C-81B7-8881D7D5F3CA}"/>
     <hyperlink ref="H1" r:id="rId6" display="https://www.amazon.com/Yohii-Position-Vertical-Switch-SS13F11/dp/B07DNY27QB/ref=sr_1_11?crid=37FHDP7FPF998&amp;dib=eyJ2IjoiMSJ9.TmZHZGk3Hvvx_lyV6egheLU8wpUW1gQXKpK-pVoJM0YZhkksUHUBJKWiqwUQi9bXQUORBZ2FODAFGmqAx6kqR6BlfXK0BtXjfCogJMSNTGW_MvnyhMWbwwaFqZ6fDFfCzxAb2L5atYpxXBCXKbFj6BSlr-hKSALaJ9IvesXQGrzCAYdJ6u8L8nnwryZ1bUGBm8-7ZAXqObLHUMq_ZAx0SIk7rcdBataxrNZY30aDggI.Qg3lDAXLtPyvzHrJ3-Vu5ofHJ0HbOo4L6fDoAegk49o&amp;dib_tag=se&amp;keywords=large+3+position+slide+switch&amp;qid=1732387852&amp;sprefix=large3+position+slide+switch%2Caps%2C136&amp;sr=8-11" xr:uid="{A4D9C4F5-2B3F-415B-AF42-A7DA6814405E}"/>
+    <hyperlink ref="I2" r:id="rId7" display="https://www.mouser.com/ProductDetail/E-Switch/JN2UEENAGX?qs=%252BZnE%2FxbLNR81sZ2W8kOt9Q%3D%3D" xr:uid="{1E28E210-299F-4167-810A-487F35F35F00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>